<commit_message>
+ modify 七月记录表 + add 20170724Pizza.md
</commit_message>
<xml_diff>
--- a/PK/七月记录表.xlsx
+++ b/PK/七月记录表.xlsx
@@ -46,7 +46,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="m/d;@"/>
+    <numFmt numFmtId="176" formatCode="m/d;@"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -124,13 +124,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+    <xf numFmtId="176" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -417,7 +417,7 @@
   <dimension ref="A1:R16385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -496,6 +496,9 @@
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:18">
       <c r="A4" s="1" t="s">

</xml_diff>

<commit_message>
+ finish reading 6-1
</commit_message>
<xml_diff>
--- a/PK/七月记录表.xlsx
+++ b/PK/七月记录表.xlsx
@@ -417,7 +417,7 @@
   <dimension ref="A1:R16385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -491,12 +491,21 @@
       <c r="B2">
         <v>1</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" spans="1:18">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="G3">
         <v>1</v>
       </c>
     </row>

</xml_diff>